<commit_message>
docker 1# update excel
</commit_message>
<xml_diff>
--- a/Docker/excel/jadlospis2.xlsx
+++ b/Docker/excel/jadlospis2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMOWANIE\etmeall2\EatMeAll\Docker\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CD525C-6FE9-4E67-83BF-36039E44CC0E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDE900B-643D-4C6B-8FBF-F27C063513B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{DC9E3696-05CD-4AC0-85C8-C796492A84E0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="506">
   <si>
     <t>Koktajl mleczny z otrębami</t>
   </si>
@@ -1106,6 +1106,462 @@
   </si>
   <si>
     <t>Jajko ugotuj na twardo, obierz i pokrój; Pokrój pomidora i cebulę; Dodaj obrane i pokrojone w drobną kostkę awokado. Wymieszaj; Skrop oliwą i przypraw bazylią i oregano; Podawaj z pieczywem</t>
+  </si>
+  <si>
+    <t>OWSIANKA Z MANDARYNKAMI, MIGDAŁAMI I ŻURAWINĄ</t>
+  </si>
+  <si>
+    <t>Płatki zalej niewielką ilością wrzątku i odstaw by napęczniały; Dodaj ciepłe mleko, obrane mandarynki, żurawinę oraz migdały</t>
+  </si>
+  <si>
+    <t>KANAPKI Z RUKOLĄ, POMIDOREM I MOZZARELLĄ</t>
+  </si>
+  <si>
+    <t>rukola</t>
+  </si>
+  <si>
+    <t>Chleb posmaruj masłem; Na wierzch wyłóż rukolę oraz pokrojonego pomidora i mozzarellę</t>
+  </si>
+  <si>
+    <t>BULGUR Z INDYKIEM SUSZONYMI POMIDORAMI I CUKINIĄ</t>
+  </si>
+  <si>
+    <t>mięso z piersi indyka, bez skóry</t>
+  </si>
+  <si>
+    <t>cukinia</t>
+  </si>
+  <si>
+    <t>kasza bulgur</t>
+  </si>
+  <si>
+    <t>7,69 łyżka</t>
+  </si>
+  <si>
+    <t>Ugotuj bulgur; Mięso pokrój w kostkę i wrzuć na rozgrzany olej; Po chwili dodaj posiekany czosnek oraz pokrojoną cukinię i pomidory; Dodaj niewielką ilość wody oraz przyptawy (papryka ostra, pieprz, sól, zioła
+prowanskalskie). Duś przez kilka minut; Podawaj z kaszą</t>
+  </si>
+  <si>
+    <t>Umyj jabłko i zjedz jako przekąskę</t>
+  </si>
+  <si>
+    <t>JOGURT Z RODZYNKAMI</t>
+  </si>
+  <si>
+    <t>Dodaj rodzynki do jogurtu i wymieszaj</t>
+  </si>
+  <si>
+    <t>OMLET Z SZYNKĄ, PAPRYKĄ I SZCZYPIORKIEM</t>
+  </si>
+  <si>
+    <t>mąka pszenna typ 750</t>
+  </si>
+  <si>
+    <t>grapefruit</t>
+  </si>
+  <si>
+    <t>0,8 porcji</t>
+  </si>
+  <si>
+    <t>0,29 szt.</t>
+  </si>
+  <si>
+    <t>0,08 szkl</t>
+  </si>
+  <si>
+    <t>Białka jaja ubij, dodaj żółtka, mąkę, mleko oraz sól i pieprz. Wymieszaj; Wlej masę na rozgrzany olej i podgrzewaj chwilę; Dodaj pokrojoną szynkę, paprykę i szczypiorek; Przykryj całość i podgrzewaj aż omlet całkowicie się zetnie; Posyp pokruszonym serem feta</t>
+  </si>
+  <si>
+    <t>JAJECZNICA Z BOCZKIEM I SZCZYPIORKIEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boczek wędzony </t>
+  </si>
+  <si>
+    <t>1,4 łyczeczki</t>
+  </si>
+  <si>
+    <t>0,3 porcji</t>
+  </si>
+  <si>
+    <t>0,25 szt.</t>
+  </si>
+  <si>
+    <t>Boczek drobno pokrój. Wrzuć na rozgrzany olej i podsmażaj przez chwilkę; Wbij jajka i dodaj posiekany szczypiorek; Przypraw pieprzem i odrobiną soli; Podsmażaj cały czas mieszając aż do ścięcia jajecznicy; Podawaj z pieczywem posmarowanym masłem</t>
+  </si>
+  <si>
+    <t>KANAPKI Z SZYNKĄ, RUKOLĄ I RZODKIEWKĄ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     15 szt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">X </t>
+  </si>
+  <si>
+    <t>Chleb posmaruj masłem; Na wierzch wyłóż rukolę, szynkę i pokrojoną rzodkiewkę</t>
+  </si>
+  <si>
+    <t>PĘCZAK Z KURCZAKIEM, PAPRYKĄ I MARCHEWKĄ</t>
+  </si>
+  <si>
+    <t>pomidory z puszki, krojone</t>
+  </si>
+  <si>
+    <t>kasza jęczmienna pęczak</t>
+  </si>
+  <si>
+    <t>mięso z piersi kurczaka, bez skóry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 szt. </t>
+  </si>
+  <si>
+    <t>6,67 łyżki</t>
+  </si>
+  <si>
+    <t>Kaszę ugotuj; Cebulę posiekaj i zeszklij na rozgrzanej oliwie; Dodaj po chwili pokrojoną paprykę i marchewkę; Po 5 minutach dodaj pokrojonego w kostkę i przyprawionego (chili, pieprz ziołowy)
+kurczaka; Gdy mięso się zetnie, dodaj pomidory i zioła prowansalskie. Duś kilka minut pod
+przykryciem; Wymieszaj z ugotowaną kaszą</t>
+  </si>
+  <si>
+    <t>KEFIR + BANAN</t>
+  </si>
+  <si>
+    <t>kefir</t>
+  </si>
+  <si>
+    <t>SAŁATKA Z TOFU I SŁONECZNIKIEM</t>
+  </si>
+  <si>
+    <t>słonecznik łuskany</t>
+  </si>
+  <si>
+    <t>sok cytrynowy</t>
+  </si>
+  <si>
+    <t>ogórek</t>
+  </si>
+  <si>
+    <t>tofu wędzone</t>
+  </si>
+  <si>
+    <t>5 liści</t>
+  </si>
+  <si>
+    <t>Pokrój tofu i warzywa; Dodaj liście sałaty oraz nasiona słonecznika; Całość polej sokiem z cytryny i wymieszaj; Podawaj z pieczywem z masłem</t>
+  </si>
+  <si>
+    <t>KANAPKI Z HUMMUSEM, JAJKIEM, SAŁATĄ I RZODKIEWKĄ</t>
+  </si>
+  <si>
+    <t>4 łyżeczki</t>
+  </si>
+  <si>
+    <t>Ugotuj jajko na twardo; Chleb posmaruj hummusem; Wyłóż sałatę oraz pokrojone jajko i rzodkiewkę</t>
+  </si>
+  <si>
+    <t>KANAPKI Z MASŁEM ORZECHOWYM I DŻEMEM</t>
+  </si>
+  <si>
+    <t>dżem wiśniowy, niskosłodzony</t>
+  </si>
+  <si>
+    <t>3 łyżeczki</t>
+  </si>
+  <si>
+    <t>Pieczywo posmaruj masłem orzechowym i dżemem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obiad </t>
+  </si>
+  <si>
+    <t>MAKARON ZE SZPINAKIEM, KURCZAKIEM I SEREM FETA</t>
+  </si>
+  <si>
+    <t>szpinak mrożony</t>
+  </si>
+  <si>
+    <t>pietruszka liście</t>
+  </si>
+  <si>
+    <t>1 porcja</t>
+  </si>
+  <si>
+    <t>1 ząbek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 szt. </t>
+  </si>
+  <si>
+    <t>1,86 szklanki</t>
+  </si>
+  <si>
+    <t>Ugotuj makaron; Podsmaż pokrojone w kostkę i przyprawione solą i pieprzem mięso na oliwie razem z
+wyciśniętym przez praskę czosnkiem; Po chwili dodaj szpinak i podsmaż jeszcze przez kilka minut; Dodaj pokruszony ser feta; Wymieszaj makaron ze szpinakiem; Pokrój pomidorki koktajlowe na pół i dodaj do potrawy na talerzu; Potrawę posyp pietruszką</t>
+  </si>
+  <si>
+    <t>BANAN+RODZYNKI, SUSZONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 łyżki </t>
+  </si>
+  <si>
+    <t>SAŁATKA MAKARONOWA Z KURCZAKIEM, RUKOLĄ I SUSZONYMI
+POMIDORAMI</t>
+  </si>
+  <si>
+    <t>Mięso pokrój w paski, natrzyj oliwą i przyprawami (sól, pieprz, papryka); Mięso wrzuć do garnka i zalej niewielką ilością wrzątku, gotuj przez 10 minut; Makaron ugotuj al dente; Pomidory suszone pokrój na małe kawałki; Wymieszaj wszystkie składniki; Posyp nasionami słonecznika i skrop oliwą</t>
+  </si>
+  <si>
+    <t>TWAROŻEK Z MIODEM I ORZECHAMI</t>
+  </si>
+  <si>
+    <t>miód pszczeli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cynamon </t>
+  </si>
+  <si>
+    <t>1,4 łyżeczki</t>
+  </si>
+  <si>
+    <t>0,4 łyżeczki</t>
+  </si>
+  <si>
+    <t>Ser rozgnieć widelcem i wymieszaj z jogurtem; Dodaj cynamon, posiekane orzechy oraz miód. Wymieszaj; Podawaj z pieczywem</t>
+  </si>
+  <si>
+    <t>KANAPKI Z HUMMUSEM, SAŁATĄ I SZYNKĄ</t>
+  </si>
+  <si>
+    <t>Chleb posmaruj hummusem.; Na wierzch wyłóż sałatę i szynkę</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 szt. </t>
+  </si>
+  <si>
+    <t>KURCZAK Z RYŻEM, WARZYWAMI I CURRY</t>
+  </si>
+  <si>
+    <t>groszek zielony, konserwowy</t>
+  </si>
+  <si>
+    <t>curry</t>
+  </si>
+  <si>
+    <t>2 szczypty</t>
+  </si>
+  <si>
+    <t>Ryż ugotuj i wymieszaj z curry; Na rozgrzany olej wrzuć posiekaną cebulą oraz czosnek; Po chwili dodaj pokrojone w kostkę mięso (przypraw pieprzem, solą i curry); Dodaj pokrojoną w plasterki marchewkę i paprykę; Dodaj niewielką ilość wody i duś pod przykryciem ok. 15-20 minut; Chwile przed końcem dodaj kukurydzę i groszek</t>
+  </si>
+  <si>
+    <t>Umyj jabłko i zjedz jako przekąskę.</t>
+  </si>
+  <si>
+    <t>JABŁKO+MIESZANKA STUDENCKA</t>
+  </si>
+  <si>
+    <t>SAŁATKA Z POMIDOREM, OGÓRKIEM, MAKRELĄ WĘDZONĄ I RUKOLĄ</t>
+  </si>
+  <si>
+    <t>cebula czerwona</t>
+  </si>
+  <si>
+    <t xml:space="preserve">olej lniany </t>
+  </si>
+  <si>
+    <t>makrela wędzona</t>
+  </si>
+  <si>
+    <t>0.64 szt.</t>
+  </si>
+  <si>
+    <t>Pokrój pomidora, cebulę i ogórka; Wymieszaj warzywa oraz dodaj rukolę i kawałki makreli; Dodaj olej oraz pieprz i sól. Wymieszaj; Podawaj z pieczywem z masłem</t>
+  </si>
+  <si>
+    <t>OMLET OWSIANY Z MASŁEM ORZECHOWYM I BANANEM</t>
+  </si>
+  <si>
+    <t>0,3 łyżeczki</t>
+  </si>
+  <si>
+    <t>Jaja rozbij, dodaj łyżkę wody lub mleka oraz płatki. Przypraw pieprzem i solą i
+wymieszaj dokładnie; Patelnię przesmaruj olejem i wlej masę jajeczną. Omlet obsmaż z obu stron (gdy jedna
+strona się zarumieni możesz zsunąć omlet na talerz i przewrócić na drugą stronę); Omlet posmaruj masłem orzechowym. Na wierzch ułóż pokrojonego w plastry banana
+(możesz posypać cynamonem)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lunch </t>
+  </si>
+  <si>
+    <t>KANAPKI Z SZYNKĄ, MUSZTARDĄ, POMIDOREM I OGÓRKIEM KISZONYM</t>
+  </si>
+  <si>
+    <t>musztarda</t>
+  </si>
+  <si>
+    <t>Chleb posmaruj masłem i musztardą; Na wierzch wyłóż szynkę, pokrojonego pomidora i ogórka</t>
+  </si>
+  <si>
+    <t>INDYK Z WARZYWAMI, SOSEM SOJOWYM I KUSKUSEMkuskus</t>
+  </si>
+  <si>
+    <t>sos sojowy ciemny</t>
+  </si>
+  <si>
+    <t>8,33 łyżki</t>
+  </si>
+  <si>
+    <t>Mięso pokrój w kostkę, natrzyj olejem oraz pieprzem i chili; Warzywa i pieczarki pokrój i wrzuć na patelnie, zalej niewielką ilością wody. Dodaj sos
+sojowy i duś kilka minut; Dodaj mięso i duś do czasu aż warzywa będą miękkie, a mięso ugotowane (w razie
+potrzeby dolewaj wody); Podawaj z przygotowanym kuskusem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">przekąska </t>
+  </si>
+  <si>
+    <t>JOGURT Z PŁATKAMI KUKURYDZIANYMI I NASIONAMI SŁONECZNIKA</t>
+  </si>
+  <si>
+    <t>płatki kukurydziane</t>
+  </si>
+  <si>
+    <t>10 łyżek</t>
+  </si>
+  <si>
+    <t>Wymieszaj razem składniki i zjedz.</t>
+  </si>
+  <si>
+    <t>TWAROŻEK Z RZODKIEWKĄ I SZCZYPIORKIEM + KANAPKI Z HUMMUSEM I PAPRYKĄ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 szt. </t>
+  </si>
+  <si>
+    <t>3 łyżki</t>
+  </si>
+  <si>
+    <t>0,43 szt.</t>
+  </si>
+  <si>
+    <t>Rozdrobnij widelcem twaróg i wymieszaj z twarogiem; Dodaj pokrojoną rzodkiewkę i posiekany szczypiorek.; Dopraw serek za pomocą ziół i pieprzu</t>
+  </si>
+  <si>
+    <t>Chleb posmaruj hummusem.; Na kanapki wyłóż pokrojoną paprykę</t>
+  </si>
+  <si>
+    <t>PLACKI Z SERKA WIEJSKIEGO Z DŻEMEM</t>
+  </si>
+  <si>
+    <t>dżem truskawowy, niskosłodzony</t>
+  </si>
+  <si>
+    <t>cukier wanilinowy</t>
+  </si>
+  <si>
+    <t>0,5 łyżeczki</t>
+  </si>
+  <si>
+    <t>3,33 łyżka</t>
+  </si>
+  <si>
+    <t>Białka jaj oddziel od żółtek i ubij na sztywną pianę; Wymieszaj żółtka, mąkę, serek, cukier i olej. Na koniec dodaj sztywną pianę z białka i
+delikatnie wymieszaj; Uformuj placki z otrzymanej masy na rozgrzanej patelni teflonowej bez użycia tłuszczu.
+Obsmaż obu stron; Posmaruj dżemem</t>
+  </si>
+  <si>
+    <t>KOKTAJL BANANOWO-POMARAŃCZOWY</t>
+  </si>
+  <si>
+    <t>BURGER WOŁOWY Z RUKOLĄ</t>
+  </si>
+  <si>
+    <t>bułki grahamki</t>
+  </si>
+  <si>
+    <t>2 garście</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zmiel mięso i przypraw solą oraz pieprzem; Mięso wyrabiaj ręką i uformuj płaski kotlet; Mięso możesz usmażyć na mocno rozgrzanej patelni grillowej bez użycia tłuszczu (po ok
+3 minuty z każdej strony) lub wstawić do piekarnika i piec ok. 15 minut; Bułkę przekrój na pół i zapiecz w tosterze lub piekarniku; Ba ciepłą bułkę wyłóż rukolę mięso, musztardę, ketchup oraz pokrojonego ogórka,
+pomidora i cebulę. Przykryj drugą połówką bułki </t>
+  </si>
+  <si>
+    <t>KANAPKI Z MAKRELĄ WĘDZONĄ, MUSZTARDĄ I POMIDOREM</t>
+  </si>
+  <si>
+    <t>0,64 szt.</t>
+  </si>
+  <si>
+    <t>Posmaruj pieczywo masłem; Kanapkę posmaruj musztardą; Na wierzch ułóż plastry pomidora i kawałki makreli</t>
+  </si>
+  <si>
+    <t>NALEŚNIKI Z JOGURTEM I KAKI</t>
+  </si>
+  <si>
+    <t>kaki</t>
+  </si>
+  <si>
+    <t>jogurt grecki</t>
+  </si>
+  <si>
+    <t>woda</t>
+  </si>
+  <si>
+    <t>0.5 szt.</t>
+  </si>
+  <si>
+    <t>Do mleka dodaj taką samą ilość wody; Wbij jaja i wymieszaj; Dodaj mąkę i wymieszaj; Patelnię delikatnie wysmaruj olejem i wlewaj ciasto naleśnikowe. Usmaż z obu stron; Naleśniki posmaruj jogurtem i wyłóż pokrojone kaki. Zwiń</t>
+  </si>
+  <si>
+    <t>KOKTAJL BANANOWO-TRUSKAWKOWY</t>
+  </si>
+  <si>
+    <t>truskawki mrożone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 łyżki </t>
+  </si>
+  <si>
+    <t>RYBA PIECZONA Z PAPRYKĄ I MOZZARELLĄ</t>
+  </si>
+  <si>
+    <t>brokuły mrożone</t>
+  </si>
+  <si>
+    <t>oliwki czarne</t>
+  </si>
+  <si>
+    <t>zioła prowansaldzkie</t>
+  </si>
+  <si>
+    <t>0,44 opakowania</t>
+  </si>
+  <si>
+    <t>0,36 szt.</t>
+  </si>
+  <si>
+    <t>0,33 łyżeczki</t>
+  </si>
+  <si>
+    <t>Rybę oprósz pieprzem i odrobiną soli. Skrop olejem; Paprykę drobno pokrój i posyp nią rybę; Na wierzch połóż mozzarellę i pokrojone oliwki. Posyp ziołami; Zawiń w folię do pieczenia i wstaw do piekarnika (200 stopni) na 20 minut. 5 minut
+przed końcem pieczenia rozwiń folię; Podawaj z ugotowanymi ziemniakami i brokulami</t>
+  </si>
+  <si>
+    <t>JOGURT Z MUSLI</t>
+  </si>
+  <si>
+    <t>Wymieszaj jogurt z musli</t>
+  </si>
+  <si>
+    <t>SAŁATKA Z POMIDOREM, OGÓRKIEM, SAŁATĄ I MOZZARELLĄsałata</t>
+  </si>
+  <si>
+    <t>3 liście</t>
+  </si>
+  <si>
+    <t>Pokrój pomidora, cebulę i ogórka; Wymieszaj warzywa oraz dodaj porwane na mniejsze części liście sałaty; Dodaj kawałki mozzarelli, oliwę oraz pieprz i sól. Wymieszaj; Podawaj z pieczywem z masłem</t>
   </si>
 </sst>
 </file>
@@ -1154,7 +1610,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1177,11 +1633,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1190,6 +1675,30 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1504,10 +2013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1838D449-8DD4-4711-984B-E0AC88629B5C}">
-  <dimension ref="A1:K374"/>
+  <dimension ref="A1:K615"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F344" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I364" sqref="I364"/>
+    <sheetView tabSelected="1" topLeftCell="A348" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A616" sqref="A616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9691,17 +10200,37 @@
       <c r="J370" s="1"/>
       <c r="K370" s="1"/>
     </row>
-    <row r="371" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A371" s="1"/>
-      <c r="B371" s="1"/>
-      <c r="C371" s="1"/>
-      <c r="D371" s="1"/>
-      <c r="E371" s="1"/>
-      <c r="F371" s="1"/>
-      <c r="G371" s="1"/>
-      <c r="H371" s="1"/>
-      <c r="I371" s="1"/>
-      <c r="J371" s="1"/>
+    <row r="371" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A371" s="1">
+        <v>64</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C371" s="1">
+        <v>10</v>
+      </c>
+      <c r="D371" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E371" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F371" s="1">
+        <v>50</v>
+      </c>
+      <c r="G371" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H371" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="I371" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="J371" s="1">
+        <v>629</v>
+      </c>
       <c r="K371" s="1"/>
     </row>
     <row r="372" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9709,10 +10238,18 @@
       <c r="B372" s="1"/>
       <c r="C372" s="1"/>
       <c r="D372" s="1"/>
-      <c r="E372" s="1"/>
-      <c r="F372" s="1"/>
-      <c r="G372" s="1"/>
-      <c r="H372" s="1"/>
+      <c r="E372" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F372" s="1">
+        <v>24</v>
+      </c>
+      <c r="G372" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H372" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I372" s="1"/>
       <c r="J372" s="1"/>
       <c r="K372" s="1"/>
@@ -9722,10 +10259,18 @@
       <c r="B373" s="1"/>
       <c r="C373" s="1"/>
       <c r="D373" s="1"/>
-      <c r="E373" s="1"/>
-      <c r="F373" s="1"/>
-      <c r="G373" s="1"/>
-      <c r="H373" s="1"/>
+      <c r="E373" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F373" s="1">
+        <v>130</v>
+      </c>
+      <c r="G373" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H373" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="I373" s="1"/>
       <c r="J373" s="1"/>
       <c r="K373" s="1"/>
@@ -9735,13 +10280,3973 @@
       <c r="B374" s="1"/>
       <c r="C374" s="1"/>
       <c r="D374" s="1"/>
-      <c r="E374" s="1"/>
-      <c r="F374" s="1"/>
-      <c r="G374" s="1"/>
-      <c r="H374" s="1"/>
+      <c r="E374" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F374" s="1">
+        <v>250</v>
+      </c>
+      <c r="G374" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H374" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="I374" s="1"/>
       <c r="J374" s="1"/>
       <c r="K374" s="1"/>
+    </row>
+    <row r="375" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A375" s="1"/>
+      <c r="B375" s="1"/>
+      <c r="C375" s="1"/>
+      <c r="D375" s="1"/>
+      <c r="E375" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F375" s="1">
+        <v>30</v>
+      </c>
+      <c r="G375" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H375" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I375" s="1"/>
+      <c r="J375" s="1"/>
+      <c r="K375" s="1"/>
+    </row>
+    <row r="376" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A376" s="1"/>
+      <c r="B376" s="1"/>
+      <c r="C376" s="1"/>
+      <c r="D376" s="1"/>
+      <c r="E376" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F376" s="1"/>
+      <c r="G376" s="1"/>
+      <c r="H376" s="1"/>
+      <c r="I376" s="1"/>
+      <c r="J376" s="1"/>
+      <c r="K376" s="1"/>
+    </row>
+    <row r="377" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A377" s="1">
+        <v>65</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C377" s="1">
+        <v>5</v>
+      </c>
+      <c r="D377" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E377" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="F377" s="1">
+        <v>10</v>
+      </c>
+      <c r="G377" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H377" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I377" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="J377" s="1">
+        <v>618</v>
+      </c>
+      <c r="K377" s="1"/>
+    </row>
+    <row r="378" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A378" s="1"/>
+      <c r="B378" s="1"/>
+      <c r="C378" s="1"/>
+      <c r="D378" s="1"/>
+      <c r="E378" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F378" s="1">
+        <v>120</v>
+      </c>
+      <c r="G378" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H378" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I378" s="1"/>
+      <c r="J378" s="1"/>
+      <c r="K378" s="1"/>
+    </row>
+    <row r="379" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A379" s="1"/>
+      <c r="B379" s="1"/>
+      <c r="C379" s="1"/>
+      <c r="D379" s="1"/>
+      <c r="E379" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F379" s="1">
+        <v>120</v>
+      </c>
+      <c r="G379" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H379" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I379" s="1"/>
+      <c r="J379" s="1"/>
+      <c r="K379" s="1"/>
+    </row>
+    <row r="380" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A380" s="1"/>
+      <c r="B380" s="1"/>
+      <c r="C380" s="1"/>
+      <c r="D380" s="1"/>
+      <c r="E380" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F380" s="1">
+        <v>20</v>
+      </c>
+      <c r="G380" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H380" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="I380" s="1"/>
+      <c r="J380" s="1"/>
+      <c r="K380" s="1"/>
+    </row>
+    <row r="381" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A381" s="1"/>
+      <c r="B381" s="1"/>
+      <c r="C381" s="1"/>
+      <c r="D381" s="1"/>
+      <c r="E381" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F381" s="1">
+        <v>60</v>
+      </c>
+      <c r="G381" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H381" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="I381" s="1"/>
+      <c r="J381" s="1"/>
+      <c r="K381" s="1"/>
+    </row>
+    <row r="382" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A382" s="1"/>
+      <c r="B382" s="1"/>
+      <c r="C382" s="1"/>
+      <c r="D382" s="1"/>
+      <c r="E382" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F382" s="1">
+        <v>150</v>
+      </c>
+      <c r="G382" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H382" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I382" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="J382" s="1"/>
+      <c r="K382" s="1"/>
+    </row>
+    <row r="383" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A383" s="1"/>
+      <c r="B383" s="1"/>
+      <c r="C383" s="1"/>
+      <c r="D383" s="1"/>
+      <c r="E383" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F383" s="1"/>
+      <c r="G383" s="1"/>
+      <c r="H383" s="1"/>
+      <c r="I383" s="1"/>
+      <c r="J383" s="1"/>
+      <c r="K383" s="1"/>
+    </row>
+    <row r="384" spans="1:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A384" s="1">
+        <v>66</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C384" s="1">
+        <v>30</v>
+      </c>
+      <c r="D384" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E384" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="F384" s="1">
+        <v>200</v>
+      </c>
+      <c r="G384" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H384" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I384" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="J384" s="1">
+        <v>859</v>
+      </c>
+      <c r="K384" s="1"/>
+    </row>
+    <row r="385" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A385" s="1"/>
+      <c r="B385" s="1"/>
+      <c r="C385" s="1"/>
+      <c r="D385" s="1"/>
+      <c r="E385" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F385" s="1">
+        <v>10</v>
+      </c>
+      <c r="G385" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H385" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I385" s="1"/>
+      <c r="J385" s="1"/>
+      <c r="K385" s="1"/>
+    </row>
+    <row r="386" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A386" s="1"/>
+      <c r="B386" s="1"/>
+      <c r="C386" s="1"/>
+      <c r="D386" s="1"/>
+      <c r="E386" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="F386" s="1">
+        <v>150</v>
+      </c>
+      <c r="G386" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H386" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I386" s="1"/>
+      <c r="J386" s="1"/>
+      <c r="K386" s="1"/>
+    </row>
+    <row r="387" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A387" s="1"/>
+      <c r="B387" s="1"/>
+      <c r="C387" s="1"/>
+      <c r="D387" s="1"/>
+      <c r="E387" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F387" s="1">
+        <v>3</v>
+      </c>
+      <c r="G387" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H387" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="I387" s="1"/>
+      <c r="J387" s="1"/>
+      <c r="K387" s="1"/>
+    </row>
+    <row r="388" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A388" s="1"/>
+      <c r="B388" s="1"/>
+      <c r="C388" s="1"/>
+      <c r="D388" s="1"/>
+      <c r="E388" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F388" s="1">
+        <v>3</v>
+      </c>
+      <c r="G388" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H388" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="I388" s="1"/>
+      <c r="J388" s="1"/>
+      <c r="K388" s="1"/>
+    </row>
+    <row r="389" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A389" s="1"/>
+      <c r="B389" s="1"/>
+      <c r="C389" s="1"/>
+      <c r="D389" s="1"/>
+      <c r="E389" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F389" s="1">
+        <v>100</v>
+      </c>
+      <c r="G389" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H389" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="I389" s="1"/>
+      <c r="J389" s="1"/>
+      <c r="K389" s="1"/>
+    </row>
+    <row r="390" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A390" s="1"/>
+      <c r="B390" s="1"/>
+      <c r="C390" s="1"/>
+      <c r="D390" s="1"/>
+      <c r="E390" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F390" s="1">
+        <v>250</v>
+      </c>
+      <c r="G390" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H390" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I390" s="1"/>
+      <c r="J390" s="1"/>
+      <c r="K390" s="1"/>
+    </row>
+    <row r="391" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A391" s="1"/>
+      <c r="B391" s="1"/>
+      <c r="C391" s="1"/>
+      <c r="D391" s="1"/>
+      <c r="E391" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F391" s="1">
+        <v>260</v>
+      </c>
+      <c r="G391" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H391" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="I391" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J391" s="1"/>
+      <c r="K391" s="1"/>
+    </row>
+    <row r="392" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A392" s="1"/>
+      <c r="B392" s="1"/>
+      <c r="C392" s="1"/>
+      <c r="D392" s="1"/>
+      <c r="E392" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F392" s="1"/>
+      <c r="G392" s="1"/>
+      <c r="H392" s="1"/>
+      <c r="I392" s="1"/>
+      <c r="J392" s="1"/>
+      <c r="K392" s="1"/>
+    </row>
+    <row r="393" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A393" s="1">
+        <v>67</v>
+      </c>
+      <c r="B393" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C393" s="1">
+        <v>5</v>
+      </c>
+      <c r="D393" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E393" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F393" s="1">
+        <v>60</v>
+      </c>
+      <c r="G393" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H393" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I393" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="J393" s="1">
+        <v>279</v>
+      </c>
+      <c r="K393" s="1"/>
+    </row>
+    <row r="394" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A394" s="1"/>
+      <c r="B394" s="1"/>
+      <c r="C394" s="1"/>
+      <c r="D394" s="1"/>
+      <c r="E394" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F394" s="1">
+        <v>180</v>
+      </c>
+      <c r="G394" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H394" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I394" s="1"/>
+      <c r="J394" s="1"/>
+      <c r="K394" s="1"/>
+    </row>
+    <row r="395" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A395" s="1"/>
+      <c r="B395" s="1"/>
+      <c r="C395" s="1"/>
+      <c r="D395" s="1"/>
+      <c r="E395" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F395" s="1"/>
+      <c r="G395" s="1"/>
+      <c r="H395" s="1"/>
+      <c r="I395" s="1"/>
+      <c r="J395" s="1"/>
+      <c r="K395" s="1"/>
+    </row>
+    <row r="396" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A396" s="1">
+        <v>68</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C396" s="1">
+        <v>15</v>
+      </c>
+      <c r="D396" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E396" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F396" s="1">
+        <v>40</v>
+      </c>
+      <c r="G396" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H396" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="I396" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="J396" s="1">
+        <v>573</v>
+      </c>
+      <c r="K396" s="1"/>
+    </row>
+    <row r="397" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A397" s="1"/>
+      <c r="B397" s="1"/>
+      <c r="C397" s="1"/>
+      <c r="D397" s="1"/>
+      <c r="E397" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F397" s="1">
+        <v>5</v>
+      </c>
+      <c r="G397" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H397" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="I397" s="1"/>
+      <c r="J397" s="1"/>
+      <c r="K397" s="1"/>
+    </row>
+    <row r="398" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A398" s="1"/>
+      <c r="B398" s="1"/>
+      <c r="C398" s="1"/>
+      <c r="D398" s="1"/>
+      <c r="E398" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F398" s="1">
+        <v>40</v>
+      </c>
+      <c r="G398" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H398" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="I398" s="1"/>
+      <c r="J398" s="1"/>
+      <c r="K398" s="1"/>
+    </row>
+    <row r="399" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A399" s="1"/>
+      <c r="B399" s="1"/>
+      <c r="C399" s="1"/>
+      <c r="D399" s="1"/>
+      <c r="E399" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F399" s="1">
+        <v>3</v>
+      </c>
+      <c r="G399" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H399" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="I399" s="1"/>
+      <c r="J399" s="1"/>
+      <c r="K399" s="1"/>
+    </row>
+    <row r="400" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A400" s="1"/>
+      <c r="B400" s="1"/>
+      <c r="C400" s="1"/>
+      <c r="D400" s="1"/>
+      <c r="E400" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F400" s="1">
+        <v>45</v>
+      </c>
+      <c r="G400" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H400" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="I400" s="1"/>
+      <c r="J400" s="1"/>
+      <c r="K400" s="1"/>
+    </row>
+    <row r="401" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A401" s="1"/>
+      <c r="B401" s="1"/>
+      <c r="C401" s="1"/>
+      <c r="D401" s="1"/>
+      <c r="E401" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="F401" s="1">
+        <v>15</v>
+      </c>
+      <c r="G401" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H401" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I401" s="1"/>
+      <c r="J401" s="1"/>
+      <c r="K401" s="1"/>
+    </row>
+    <row r="402" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A402" s="1"/>
+      <c r="B402" s="1"/>
+      <c r="C402" s="1"/>
+      <c r="D402" s="1"/>
+      <c r="E402" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F402" s="1">
+        <v>20</v>
+      </c>
+      <c r="G402" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H402" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="I402" s="1"/>
+      <c r="J402" s="1"/>
+      <c r="K402" s="1"/>
+    </row>
+    <row r="403" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A403" s="1"/>
+      <c r="B403" s="1"/>
+      <c r="C403" s="1"/>
+      <c r="D403" s="1"/>
+      <c r="E403" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F403" s="1">
+        <v>168</v>
+      </c>
+      <c r="G403" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H403" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I403" s="1"/>
+      <c r="J403" s="1"/>
+      <c r="K403" s="1"/>
+    </row>
+    <row r="404" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A404" s="1"/>
+      <c r="B404" s="1"/>
+      <c r="C404" s="1"/>
+      <c r="D404" s="1"/>
+      <c r="E404" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="F404" s="1">
+        <v>220</v>
+      </c>
+      <c r="G404" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H404" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I404" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J404" s="1"/>
+      <c r="K404" s="1"/>
+    </row>
+    <row r="405" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A405" s="1"/>
+      <c r="B405" s="1"/>
+      <c r="C405" s="1"/>
+      <c r="D405" s="1"/>
+      <c r="E405" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F405" s="1"/>
+      <c r="G405" s="1"/>
+      <c r="H405" s="1"/>
+      <c r="I405" s="1"/>
+      <c r="J405" s="1"/>
+      <c r="K405" s="1"/>
+    </row>
+    <row r="406" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A406" s="1">
+        <v>69</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C406" s="1">
+        <v>15</v>
+      </c>
+      <c r="D406" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="E406" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F406" s="1">
+        <v>7</v>
+      </c>
+      <c r="G406" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H406" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="I406" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="J406" s="1">
+        <v>624</v>
+      </c>
+      <c r="K406" s="1"/>
+    </row>
+    <row r="407" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A407" s="1"/>
+      <c r="B407" s="1"/>
+      <c r="C407" s="1"/>
+      <c r="D407" s="1"/>
+      <c r="E407" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F407" s="1">
+        <v>90</v>
+      </c>
+      <c r="G407" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H407" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I407" s="1"/>
+      <c r="J407" s="1"/>
+      <c r="K407" s="1"/>
+    </row>
+    <row r="408" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A408" s="1"/>
+      <c r="B408" s="1"/>
+      <c r="C408" s="1"/>
+      <c r="D408" s="1"/>
+      <c r="E408" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="F408" s="1">
+        <v>30</v>
+      </c>
+      <c r="G408" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H408" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="I408" s="1"/>
+      <c r="J408" s="1"/>
+      <c r="K408" s="1"/>
+    </row>
+    <row r="409" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A409" s="1"/>
+      <c r="B409" s="1"/>
+      <c r="C409" s="1"/>
+      <c r="D409" s="1"/>
+      <c r="E409" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F409" s="1">
+        <v>5</v>
+      </c>
+      <c r="G409" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H409" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="I409" s="1"/>
+      <c r="J409" s="1"/>
+      <c r="K409" s="1"/>
+    </row>
+    <row r="410" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A410" s="1"/>
+      <c r="B410" s="1"/>
+      <c r="C410" s="1"/>
+      <c r="D410" s="1"/>
+      <c r="E410" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F410" s="1">
+        <v>25</v>
+      </c>
+      <c r="G410" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H410" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="I410" s="1"/>
+      <c r="J410" s="1"/>
+      <c r="K410" s="1"/>
+    </row>
+    <row r="411" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A411" s="1"/>
+      <c r="B411" s="1"/>
+      <c r="C411" s="1"/>
+      <c r="D411" s="1"/>
+      <c r="E411" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F411" s="1">
+        <v>3</v>
+      </c>
+      <c r="G411" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H411" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="I411" s="1"/>
+      <c r="J411" s="1"/>
+      <c r="K411" s="1"/>
+    </row>
+    <row r="412" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A412" s="1"/>
+      <c r="B412" s="1"/>
+      <c r="C412" s="1"/>
+      <c r="D412" s="1"/>
+      <c r="E412" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F412" s="1">
+        <v>168</v>
+      </c>
+      <c r="G412" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H412" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I412" s="1"/>
+      <c r="J412" s="1"/>
+      <c r="K412" s="1"/>
+    </row>
+    <row r="413" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A413" s="1"/>
+      <c r="B413" s="1"/>
+      <c r="C413" s="1"/>
+      <c r="D413" s="1"/>
+      <c r="E413" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F413" s="1"/>
+      <c r="G413" s="1"/>
+      <c r="H413" s="1"/>
+      <c r="I413" s="1"/>
+      <c r="J413" s="1"/>
+      <c r="K413" s="1"/>
+    </row>
+    <row r="414" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A414" s="1">
+        <v>70</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C414" s="1">
+        <v>5</v>
+      </c>
+      <c r="D414" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E414" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F414" s="1">
+        <v>10</v>
+      </c>
+      <c r="G414" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H414" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I414" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="J414" s="1">
+        <v>638</v>
+      </c>
+      <c r="K414" s="1"/>
+    </row>
+    <row r="415" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A415" s="1"/>
+      <c r="B415" s="1"/>
+      <c r="C415" s="1"/>
+      <c r="D415" s="1"/>
+      <c r="E415" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F415" s="1">
+        <v>60</v>
+      </c>
+      <c r="G415" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H415" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I415" s="1"/>
+      <c r="J415" s="1"/>
+      <c r="K415" s="1"/>
+    </row>
+    <row r="416" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E416" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F416" s="4">
+        <v>120</v>
+      </c>
+      <c r="G416" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H416" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="417" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E417" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F417" s="4">
+        <v>60</v>
+      </c>
+      <c r="G417" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H417" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="418" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E418" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="F418" s="4">
+        <v>20</v>
+      </c>
+      <c r="G418" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H418" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="419" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E419" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F419" s="4">
+        <v>75</v>
+      </c>
+      <c r="G419" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H419" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="I419" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="420" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E420" s="4" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="421" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A421">
+        <v>71</v>
+      </c>
+      <c r="B421" t="s">
+        <v>64</v>
+      </c>
+      <c r="C421">
+        <v>30</v>
+      </c>
+      <c r="D421" t="s">
+        <v>390</v>
+      </c>
+      <c r="E421" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F421" s="6">
+        <v>10</v>
+      </c>
+      <c r="G421" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H421" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I421" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="J421">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="422" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E422" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F422" s="6">
+        <v>200</v>
+      </c>
+      <c r="G422" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H422" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="423" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E423" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F423" s="6">
+        <v>50</v>
+      </c>
+      <c r="G423" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H423" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="424" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E424" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F424" s="6">
+        <v>45</v>
+      </c>
+      <c r="G424" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H424" s="7" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="425" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E425" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F425" s="6">
+        <v>100</v>
+      </c>
+      <c r="G425" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H425" s="7" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="426" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E426" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="F426" s="6">
+        <v>200</v>
+      </c>
+      <c r="G426" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H426" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="427" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E427" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F427" s="6">
+        <v>70</v>
+      </c>
+      <c r="G427" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H427" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="428" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E428" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="F428" s="6">
+        <v>250</v>
+      </c>
+      <c r="G428" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H428" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="429" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E429" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="F429" s="6">
+        <v>200</v>
+      </c>
+      <c r="G429" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H429" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="I429" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="430" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E430" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="431" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A431">
+        <v>72</v>
+      </c>
+      <c r="B431" t="s">
+        <v>174</v>
+      </c>
+      <c r="D431" t="s">
+        <v>397</v>
+      </c>
+      <c r="E431" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="F431" s="6">
+        <v>250</v>
+      </c>
+      <c r="G431" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H431" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="I431" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J431">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="432" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E432" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F432" s="6">
+        <v>120</v>
+      </c>
+      <c r="G432" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H432" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="I432" s="7"/>
+    </row>
+    <row r="433" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E433" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="434" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A434">
+        <v>73</v>
+      </c>
+      <c r="B434" t="s">
+        <v>96</v>
+      </c>
+      <c r="C434">
+        <v>10</v>
+      </c>
+      <c r="D434" t="s">
+        <v>399</v>
+      </c>
+      <c r="E434" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="F434" s="6">
+        <v>7</v>
+      </c>
+      <c r="G434" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H434" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="I434" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="J434">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="435" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E435" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F435" s="6">
+        <v>90</v>
+      </c>
+      <c r="G435" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H435" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="436" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E436" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="F436" s="6">
+        <v>20</v>
+      </c>
+      <c r="G436" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H436" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="437" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E437" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F437" s="6">
+        <v>6</v>
+      </c>
+      <c r="G437" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H437" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="438" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E438" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="F438" s="6">
+        <v>80</v>
+      </c>
+      <c r="G438" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H438" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="439" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E439" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F439" s="6">
+        <v>70</v>
+      </c>
+      <c r="G439" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H439" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="440" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E440" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F440" s="6">
+        <v>25</v>
+      </c>
+      <c r="G440" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H440" s="7" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="441" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E441" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="F441" s="6">
+        <v>90</v>
+      </c>
+      <c r="G441" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H441" s="7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="442" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E442" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F442" s="6">
+        <v>250</v>
+      </c>
+      <c r="G442" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H442" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="443" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E443" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="444" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A444">
+        <v>74</v>
+      </c>
+      <c r="B444" t="s">
+        <v>123</v>
+      </c>
+      <c r="C444">
+        <v>10</v>
+      </c>
+      <c r="D444" t="s">
+        <v>406</v>
+      </c>
+      <c r="E444" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F444" s="6">
+        <v>20</v>
+      </c>
+      <c r="G444" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H444" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I444" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="J444">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="445" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E445" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F445" s="6">
+        <v>112</v>
+      </c>
+      <c r="G445" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H445" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="446" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E446" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F446" s="6">
+        <v>60</v>
+      </c>
+      <c r="G446" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H446" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="447" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E447" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F447" s="6">
+        <v>40</v>
+      </c>
+      <c r="G447" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H447" s="7" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="448" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E448" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F448" s="6">
+        <v>120</v>
+      </c>
+      <c r="G448" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H448" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="449" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E449" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="450" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A450">
+        <v>75</v>
+      </c>
+      <c r="B450" t="s">
+        <v>63</v>
+      </c>
+      <c r="C450">
+        <v>5</v>
+      </c>
+      <c r="D450" t="s">
+        <v>409</v>
+      </c>
+      <c r="E450" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F450" s="6">
+        <v>45</v>
+      </c>
+      <c r="G450" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H450" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="I450" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="J450">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="451" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E451" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F451" s="6">
+        <v>90</v>
+      </c>
+      <c r="G451" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H451" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="452" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E452" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="F452" s="6">
+        <v>45</v>
+      </c>
+      <c r="G452" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H452" s="7" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="453" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E453" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="454" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A454">
+        <v>76</v>
+      </c>
+      <c r="B454" t="s">
+        <v>413</v>
+      </c>
+      <c r="C454">
+        <v>25</v>
+      </c>
+      <c r="D454" t="s">
+        <v>414</v>
+      </c>
+      <c r="E454" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="F454" s="6">
+        <v>200</v>
+      </c>
+      <c r="G454" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H454" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="I454" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="J454">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="455" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E455" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="F455" s="6">
+        <v>50</v>
+      </c>
+      <c r="G455" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H455" s="7" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="456" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E456" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F456" s="6">
+        <v>5</v>
+      </c>
+      <c r="G456" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H456" s="7" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="457" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E457" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="F457" s="6">
+        <v>200</v>
+      </c>
+      <c r="G457" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H457" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="458" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E458" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F458" s="6">
+        <v>5</v>
+      </c>
+      <c r="G458" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H458" s="7" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="459" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E459" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F459" s="6">
+        <v>100</v>
+      </c>
+      <c r="G459" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H459" s="7" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="460" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E460" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="F460" s="6">
+        <v>12</v>
+      </c>
+      <c r="G460" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H460" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="461" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E461" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F461" s="6">
+        <v>130</v>
+      </c>
+      <c r="G461" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H461" s="7" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="462" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E462" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="463" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A463">
+        <v>77</v>
+      </c>
+      <c r="B463" t="s">
+        <v>174</v>
+      </c>
+      <c r="D463" t="s">
+        <v>422</v>
+      </c>
+      <c r="E463" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F463" s="6">
+        <v>120</v>
+      </c>
+      <c r="G463" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H463" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I463" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J463">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="464" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E464" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="F464" s="6">
+        <v>60</v>
+      </c>
+      <c r="G464" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H464" s="7" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="465" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E465" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="466" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A466">
+        <v>78</v>
+      </c>
+      <c r="B466" t="s">
+        <v>96</v>
+      </c>
+      <c r="C466">
+        <v>25</v>
+      </c>
+      <c r="D466" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="E466" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F466" s="6">
+        <v>70</v>
+      </c>
+      <c r="G466" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H466" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I466" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="J466">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="467" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E467" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="F467" s="6">
+        <v>20</v>
+      </c>
+      <c r="G467" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H467" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="468" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E468" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="F468" s="6">
+        <v>150</v>
+      </c>
+      <c r="G468" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H468" s="7" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="469" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E469" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F469" s="6">
+        <v>10</v>
+      </c>
+      <c r="G469" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H469" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="470" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E470" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="F470" s="6">
+        <v>10</v>
+      </c>
+      <c r="G470" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H470" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="471" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E471" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F471" s="6">
+        <v>30</v>
+      </c>
+      <c r="G471" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H471" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="472" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E472" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="473" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A473">
+        <v>79</v>
+      </c>
+      <c r="B473" t="s">
+        <v>123</v>
+      </c>
+      <c r="C473">
+        <v>10</v>
+      </c>
+      <c r="D473" t="s">
+        <v>426</v>
+      </c>
+      <c r="E473" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="F473" s="6">
+        <v>7</v>
+      </c>
+      <c r="G473" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H473" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="I473" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="J473">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="474" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E474" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F474" s="6">
+        <v>90</v>
+      </c>
+      <c r="G474" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H474" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="475" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E475" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F475" s="6">
+        <v>100</v>
+      </c>
+      <c r="G475" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H475" s="7" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="476" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E476" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F476" s="6">
+        <v>100</v>
+      </c>
+      <c r="G476" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H476" s="7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="477" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E477" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="F477" s="6">
+        <v>24</v>
+      </c>
+      <c r="G477" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H477" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="478" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E478" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="F478" s="6">
+        <v>2</v>
+      </c>
+      <c r="G478" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H478" s="7" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="479" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E479" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F479" s="6">
+        <v>15</v>
+      </c>
+      <c r="G479" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H479" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="480" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E480" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="481" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A481">
+        <v>80</v>
+      </c>
+      <c r="B481" t="s">
+        <v>63</v>
+      </c>
+      <c r="C481">
+        <v>5</v>
+      </c>
+      <c r="D481" t="s">
+        <v>432</v>
+      </c>
+      <c r="E481" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F481" s="6">
+        <v>20</v>
+      </c>
+      <c r="G481" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H481" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I481" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="J481">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="482" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E482" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F482" s="6">
+        <v>120</v>
+      </c>
+      <c r="G482" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H482" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="483" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E483" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F483" s="6">
+        <v>40</v>
+      </c>
+      <c r="G483" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H483" s="7" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="484" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E484" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F484" s="6">
+        <v>60</v>
+      </c>
+      <c r="G484" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H484" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="485" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E485" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="F485" s="6">
+        <v>260</v>
+      </c>
+      <c r="G485" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H485" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="I485" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="486" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E486" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="487" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A487">
+        <v>81</v>
+      </c>
+      <c r="B487" t="s">
+        <v>64</v>
+      </c>
+      <c r="C487">
+        <v>30</v>
+      </c>
+      <c r="D487" t="s">
+        <v>435</v>
+      </c>
+      <c r="E487" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F487" s="6">
+        <v>30</v>
+      </c>
+      <c r="G487" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H487" t="s">
+        <v>17</v>
+      </c>
+      <c r="I487" t="s">
+        <v>439</v>
+      </c>
+      <c r="J487">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="488" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E488" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F488" s="6">
+        <v>70</v>
+      </c>
+      <c r="G488" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H488" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="489" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E489" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="F489" s="6">
+        <v>200</v>
+      </c>
+      <c r="G489" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H489" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="490" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E490" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="F490" s="6">
+        <v>32</v>
+      </c>
+      <c r="G490" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H490" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="491" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E491" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="F491" s="6">
+        <v>2</v>
+      </c>
+      <c r="G491" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H491" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="492" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E492" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F492" s="6">
+        <v>50</v>
+      </c>
+      <c r="G492" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H492" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="493" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E493" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F493" s="6">
+        <v>10</v>
+      </c>
+      <c r="G493" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H493" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="494" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E494" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F494" s="6">
+        <v>45</v>
+      </c>
+      <c r="G494" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H494" s="7" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="495" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E495" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F495" s="6">
+        <v>5</v>
+      </c>
+      <c r="G495" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H495" s="7" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="496" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E496" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F496" s="6">
+        <v>100</v>
+      </c>
+      <c r="G496" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H496" s="7" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="497" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E497" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F497" s="6">
+        <v>250</v>
+      </c>
+      <c r="G497" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H497" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="498" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E498" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="499" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A499">
+        <v>82</v>
+      </c>
+      <c r="B499" t="s">
+        <v>174</v>
+      </c>
+      <c r="C499">
+        <v>1</v>
+      </c>
+      <c r="D499" t="s">
+        <v>441</v>
+      </c>
+      <c r="E499" t="s">
+        <v>168</v>
+      </c>
+      <c r="F499" s="6">
+        <v>150</v>
+      </c>
+      <c r="G499" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H499" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="I499" t="s">
+        <v>440</v>
+      </c>
+      <c r="J499">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="500" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E500" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="F500" s="6">
+        <v>40</v>
+      </c>
+      <c r="G500" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H500" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="501" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E501" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="502" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A502">
+        <v>83</v>
+      </c>
+      <c r="B502" t="s">
+        <v>96</v>
+      </c>
+      <c r="C502">
+        <v>15</v>
+      </c>
+      <c r="D502" t="s">
+        <v>442</v>
+      </c>
+      <c r="E502" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="F502" s="6">
+        <v>7</v>
+      </c>
+      <c r="G502" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H502" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="I502" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="J502">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="503" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E503" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F503" s="6">
+        <v>90</v>
+      </c>
+      <c r="G503" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H503" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="504" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E504" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="F504" s="6">
+        <v>20</v>
+      </c>
+      <c r="G504" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H504" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="505" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E505" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="F505" s="6">
+        <v>30</v>
+      </c>
+      <c r="G505" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H505" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="506" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E506" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F506" s="6">
+        <v>120</v>
+      </c>
+      <c r="G506" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H506" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="507" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E507" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="F507" s="6">
+        <v>10</v>
+      </c>
+      <c r="G507" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H507" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="508" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E508" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F508" s="6">
+        <v>60</v>
+      </c>
+      <c r="G508" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H508" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="509" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E509" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="F509" s="6">
+        <v>80</v>
+      </c>
+      <c r="G509" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H509" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="510" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E510" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F510" s="6">
+        <v>250</v>
+      </c>
+      <c r="G510" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H510" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="511" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E511" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="512" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A512">
+        <v>84</v>
+      </c>
+      <c r="B512" t="s">
+        <v>123</v>
+      </c>
+      <c r="C512">
+        <v>15</v>
+      </c>
+      <c r="D512" t="s">
+        <v>448</v>
+      </c>
+      <c r="E512" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F512" s="6">
+        <v>120</v>
+      </c>
+      <c r="G512" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H512" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I512" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="J512">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="513" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E513" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="F513" s="6">
+        <v>30</v>
+      </c>
+      <c r="G513" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H513" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="514" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E514" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F514" s="6">
+        <v>3</v>
+      </c>
+      <c r="G514" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H514" s="7" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="515" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E515" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F515" s="6">
+        <v>112</v>
+      </c>
+      <c r="G515" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H515" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="516" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E516" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="F516" s="6">
+        <v>40</v>
+      </c>
+      <c r="G516" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H516" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="517" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E517" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="518" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A518">
+        <v>85</v>
+      </c>
+      <c r="B518" t="s">
+        <v>451</v>
+      </c>
+      <c r="C518">
+        <v>5</v>
+      </c>
+      <c r="D518" t="s">
+        <v>452</v>
+      </c>
+      <c r="E518" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="F518" s="6">
+        <v>10</v>
+      </c>
+      <c r="G518" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H518" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="I518" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="J518">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="519" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E519" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F519" s="6">
+        <v>60</v>
+      </c>
+      <c r="G519" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H519" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="520" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E520" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F520" s="6">
+        <v>120</v>
+      </c>
+      <c r="G520" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H520" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="521" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E521" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F521" s="6">
+        <v>120</v>
+      </c>
+      <c r="G521" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H521" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="522" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E522" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="F522" s="6">
+        <v>60</v>
+      </c>
+      <c r="G522" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H522" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="523" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E523" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="F523" s="6">
+        <v>20</v>
+      </c>
+      <c r="G523" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H523" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="524" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E524" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="F524" s="6">
+        <v>200</v>
+      </c>
+      <c r="G524" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H524" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="525" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E525" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="526" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A526">
+        <v>86</v>
+      </c>
+      <c r="B526" t="s">
+        <v>64</v>
+      </c>
+      <c r="C526">
+        <v>25</v>
+      </c>
+      <c r="D526" t="s">
+        <v>455</v>
+      </c>
+      <c r="F526" s="6">
+        <v>100</v>
+      </c>
+      <c r="G526" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H526" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="I526" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="J526">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="527" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E527" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F527" s="7">
+        <v>20</v>
+      </c>
+      <c r="G527" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H527" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="528" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E528" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F528" s="7">
+        <v>60</v>
+      </c>
+      <c r="G528" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H528" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="529" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E529" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="F529" s="7">
+        <v>150</v>
+      </c>
+      <c r="G529" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H529" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="530" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E530" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F530" s="7">
+        <v>70</v>
+      </c>
+      <c r="G530" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H530" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="531" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E531" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="F531" s="7">
+        <v>20</v>
+      </c>
+      <c r="G531" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H531" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="532" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E532" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="F532" s="7">
+        <v>200</v>
+      </c>
+      <c r="G532" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H532" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="533" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E533" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="F533" s="7">
+        <v>250</v>
+      </c>
+      <c r="G533" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H533" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="534" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E534" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="535" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A535">
+        <v>87</v>
+      </c>
+      <c r="B535" t="s">
+        <v>459</v>
+      </c>
+      <c r="C535">
+        <v>5</v>
+      </c>
+      <c r="D535" t="s">
+        <v>460</v>
+      </c>
+      <c r="E535" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="F535" s="7">
+        <v>10</v>
+      </c>
+      <c r="G535" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H535" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I535" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="J535">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="536" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E536" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="F536" s="7">
+        <v>30</v>
+      </c>
+      <c r="G536" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H536" s="7" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="537" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E537" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F537" s="7">
+        <v>200</v>
+      </c>
+      <c r="G537" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H537" s="7" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="538" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E538" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="539" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A539">
+        <v>88</v>
+      </c>
+      <c r="B539" t="s">
+        <v>96</v>
+      </c>
+      <c r="C539">
+        <v>12</v>
+      </c>
+      <c r="D539" t="s">
+        <v>464</v>
+      </c>
+      <c r="E539" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="F539" s="7">
+        <v>30</v>
+      </c>
+      <c r="G539" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H539" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="I539" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="J539">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="540" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E540" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="F540" s="7">
+        <v>100</v>
+      </c>
+      <c r="G540" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H540" s="7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="541" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E541" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F541" s="7">
+        <v>60</v>
+      </c>
+      <c r="G541" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H541" s="7" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="542" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E542" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F542" s="7">
+        <v>10</v>
+      </c>
+      <c r="G542" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H542" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="543" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E543" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F543" s="7">
+        <v>120</v>
+      </c>
+      <c r="G543" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H543" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="I543" s="7" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="544" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E544" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="F544" s="7">
+        <v>40</v>
+      </c>
+      <c r="G544" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H544" s="7" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="545" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E545" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F545" s="7">
+        <v>60</v>
+      </c>
+      <c r="G545" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H545" s="7" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="546" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E546" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="547" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A547">
+        <v>89</v>
+      </c>
+      <c r="B547" t="s">
+        <v>123</v>
+      </c>
+      <c r="C547">
+        <v>20</v>
+      </c>
+      <c r="D547" t="s">
+        <v>470</v>
+      </c>
+      <c r="E547" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="F547" s="7">
+        <v>30</v>
+      </c>
+      <c r="G547" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H547" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="I547" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="J547">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="548" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E548" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="F548" s="7">
+        <v>2</v>
+      </c>
+      <c r="G548" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H548" s="7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="549" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E549" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F549" s="7">
+        <v>10</v>
+      </c>
+      <c r="G549" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H549" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="550" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E550" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="F550" s="7">
+        <v>50</v>
+      </c>
+      <c r="G550" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H550" s="7" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="551" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E551" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F551" s="7">
+        <v>56</v>
+      </c>
+      <c r="G551" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H551" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="552" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E552" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="F552" s="7">
+        <v>200</v>
+      </c>
+      <c r="G552" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H552" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="553" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E553" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="554" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A554">
+        <v>90</v>
+      </c>
+      <c r="B554" t="s">
+        <v>63</v>
+      </c>
+      <c r="C554">
+        <v>5</v>
+      </c>
+      <c r="D554" t="s">
+        <v>476</v>
+      </c>
+      <c r="E554" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F554" s="7">
+        <v>250</v>
+      </c>
+      <c r="G554" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H554" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I554" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="J554">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="555" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E555" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="F555" s="7">
+        <v>40</v>
+      </c>
+      <c r="G555" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H555" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="556" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E556" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F556" s="7">
+        <v>120</v>
+      </c>
+      <c r="G556" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H556" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="557" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E557" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="F557" s="7">
+        <v>200</v>
+      </c>
+      <c r="G557" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H557" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="558" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E558" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="F558" s="7">
+        <v>45</v>
+      </c>
+      <c r="G558" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H558" s="7" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="559" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E559" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G559" s="7"/>
+    </row>
+    <row r="560" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A560">
+        <v>91</v>
+      </c>
+      <c r="B560" t="s">
+        <v>64</v>
+      </c>
+      <c r="C560">
+        <v>30</v>
+      </c>
+      <c r="D560" t="s">
+        <v>477</v>
+      </c>
+      <c r="E560" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="F560" s="7">
+        <v>200</v>
+      </c>
+      <c r="G560" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H560" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="I560" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="J560">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="561" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E561" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F561" s="7">
+        <v>20</v>
+      </c>
+      <c r="G561" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H561" s="7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="562" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E562" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F562" s="7">
+        <v>30</v>
+      </c>
+      <c r="G562" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H562" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="563" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E563" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="F563" s="7">
+        <v>20</v>
+      </c>
+      <c r="G563" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H563" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="564" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E564" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="F564" s="7">
+        <v>120</v>
+      </c>
+      <c r="G564" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H564" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="565" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E565" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="F565" s="7">
+        <v>130</v>
+      </c>
+      <c r="G565" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H565" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="566" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E566" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="F566" s="7">
+        <v>40</v>
+      </c>
+      <c r="G566" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H566" s="7" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="567" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E567" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F567" s="7">
+        <v>120</v>
+      </c>
+      <c r="G567" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H567" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="568" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E568" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="F568" s="7">
+        <v>250</v>
+      </c>
+      <c r="G568" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H568" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="569" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E569" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="F569" s="7">
+        <v>130</v>
+      </c>
+      <c r="G569" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H569" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I569" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="570" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E570" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="571" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A571">
+        <v>92</v>
+      </c>
+      <c r="B571" t="s">
+        <v>174</v>
+      </c>
+      <c r="D571" t="s">
+        <v>340</v>
+      </c>
+      <c r="E571" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="F571" s="7">
+        <v>60</v>
+      </c>
+      <c r="G571" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H571" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="I571" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J571">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="572" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E572" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="573" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A573">
+        <v>93</v>
+      </c>
+      <c r="B573" t="s">
+        <v>96</v>
+      </c>
+      <c r="C573">
+        <v>10</v>
+      </c>
+      <c r="D573" t="s">
+        <v>481</v>
+      </c>
+      <c r="E573" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="F573" s="7">
+        <v>20</v>
+      </c>
+      <c r="G573" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H573" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="I573" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="J573">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="574" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E574" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F574" s="9">
+        <v>120</v>
+      </c>
+      <c r="G574" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H574" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="575" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E575" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="F575" s="7">
+        <v>10</v>
+      </c>
+      <c r="G575" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H575" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="576" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E576" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="F576" s="10">
+        <v>80</v>
+      </c>
+      <c r="G576" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H576" s="9" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="577" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E577" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="F577" s="7">
+        <v>120</v>
+      </c>
+      <c r="G577" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H577" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="578" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E578" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="579" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A579">
+        <v>94</v>
+      </c>
+      <c r="B579" t="s">
+        <v>123</v>
+      </c>
+      <c r="C579">
+        <v>30</v>
+      </c>
+      <c r="D579" t="s">
+        <v>484</v>
+      </c>
+      <c r="E579" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="F579" s="9">
+        <v>125</v>
+      </c>
+      <c r="G579" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H579" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="I579" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="J579">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="580" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E580" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="F580" s="9">
+        <v>80</v>
+      </c>
+      <c r="G580" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H580" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="581" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E581" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F581" s="9">
+        <v>5</v>
+      </c>
+      <c r="G581" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H581" s="9" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="582" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E582" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F582" s="9">
+        <v>56</v>
+      </c>
+      <c r="G582" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H582" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="583" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E583" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F583" s="9">
+        <v>100</v>
+      </c>
+      <c r="G583" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H583" s="9" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="584" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E584" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="F584" s="9">
+        <v>100</v>
+      </c>
+      <c r="G584" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H584" s="9" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="585" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E585" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="F585" s="9">
+        <v>100</v>
+      </c>
+      <c r="G585" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H585" s="9" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="586" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E586" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="587" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A587">
+        <v>95</v>
+      </c>
+      <c r="B587" t="s">
+        <v>63</v>
+      </c>
+      <c r="C587">
+        <v>5</v>
+      </c>
+      <c r="D587" t="s">
+        <v>490</v>
+      </c>
+      <c r="E587" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="F587" s="9">
+        <v>30</v>
+      </c>
+      <c r="G587" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H587" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I587" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="J587">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="588" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E588" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="F588" s="9">
+        <v>30</v>
+      </c>
+      <c r="G588" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H588" s="9" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="589" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E589" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F589" s="9">
+        <v>120</v>
+      </c>
+      <c r="G589" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H589" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="590" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E590" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="F590" s="9">
+        <v>200</v>
+      </c>
+      <c r="G590" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H590" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="591" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E591" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F591" s="9">
+        <v>250</v>
+      </c>
+      <c r="G591" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H591" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="592" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E592" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G592" s="9"/>
+    </row>
+    <row r="593" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A593">
+        <v>96</v>
+      </c>
+      <c r="B593" t="s">
+        <v>64</v>
+      </c>
+      <c r="C593">
+        <v>30</v>
+      </c>
+      <c r="D593" t="s">
+        <v>493</v>
+      </c>
+      <c r="E593" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="F593" s="9">
+        <v>200</v>
+      </c>
+      <c r="G593" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H593" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="I593" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="J593">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="594" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E594" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F594" s="9">
+        <v>420</v>
+      </c>
+      <c r="G594" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H594" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="595" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E595" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F595" s="9">
+        <v>50</v>
+      </c>
+      <c r="G595" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H595" s="9" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="596" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E596" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="F596" s="9">
+        <v>15</v>
+      </c>
+      <c r="G596" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H596" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="597" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E597" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F597" s="9">
+        <v>5</v>
+      </c>
+      <c r="G597" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H597" s="9" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="598" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E598" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="F598" s="9">
+        <v>1</v>
+      </c>
+      <c r="G598" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H598" s="9" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="599" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E599" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="F599" s="9">
+        <v>45</v>
+      </c>
+      <c r="G599" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H599" s="9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="600" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E600" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="F600" s="9">
+        <v>200</v>
+      </c>
+      <c r="G600" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H600" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="601" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E601" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="F601" s="9">
+        <v>250</v>
+      </c>
+      <c r="G601" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H601" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="602" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E602" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="603" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A603">
+        <v>97</v>
+      </c>
+      <c r="B603" t="s">
+        <v>174</v>
+      </c>
+      <c r="C603">
+        <v>5</v>
+      </c>
+      <c r="D603" t="s">
+        <v>501</v>
+      </c>
+      <c r="E603" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="F603" s="9">
+        <v>50</v>
+      </c>
+      <c r="G603" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H603" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="I603" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="J603">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="604" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E604" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F604" s="9">
+        <v>180</v>
+      </c>
+      <c r="G604" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H604" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="605" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E605" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="606" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A606">
+        <v>98</v>
+      </c>
+      <c r="B606" t="s">
+        <v>96</v>
+      </c>
+      <c r="C606">
+        <v>15</v>
+      </c>
+      <c r="D606" t="s">
+        <v>503</v>
+      </c>
+      <c r="E606" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F606" s="9">
+        <v>15</v>
+      </c>
+      <c r="G606" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H606" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="I606" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="J606">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="607" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E607" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="F607" s="9">
+        <v>30</v>
+      </c>
+      <c r="G607" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H607" s="9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="608" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E608" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F608" s="9">
+        <v>120</v>
+      </c>
+      <c r="G608" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H608" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="609" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E609" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="F609" s="9">
+        <v>60</v>
+      </c>
+      <c r="G609" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H609" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="610" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E610" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="F610" s="9">
+        <v>60</v>
+      </c>
+      <c r="G610" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H610" s="9" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="611" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E611" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F611" s="9">
+        <v>10</v>
+      </c>
+      <c r="G611" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H611" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="612" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E612" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="F612" s="9">
+        <v>90</v>
+      </c>
+      <c r="G612" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H612" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="613" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E613" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="F613" s="9">
+        <v>7</v>
+      </c>
+      <c r="G613" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H613" s="9" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="614" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E614" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F614" s="9">
+        <v>250</v>
+      </c>
+      <c r="G614" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H614" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="615" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E615" s="7" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>